<commit_message>
Update DB Final #2
</commit_message>
<xml_diff>
--- a/database/Data_Dummy.xlsx
+++ b/database/Data_Dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frans Nathanael\Desktop\To Be Continued\Semester 4\PCS\Proyek\program\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29701EA8-134C-47A2-8A82-B53237B611F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E9E156-87AD-470F-9EB6-1C80312DA0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="12" xr2:uid="{103EB8D4-6D39-4DA4-B210-D1A405D40687}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3612" uniqueCount="1085">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="1091">
   <si>
     <t>kode_karyawan</t>
   </si>
@@ -3300,6 +3300,24 @@
   </si>
   <si>
     <t>248</t>
+  </si>
+  <si>
+    <t>2022-04-28</t>
+  </si>
+  <si>
+    <t>2022-05-18</t>
+  </si>
+  <si>
+    <t>2022-05-17</t>
+  </si>
+  <si>
+    <t>jadwal_check_in</t>
+  </si>
+  <si>
+    <t>jadwal_check_out</t>
+  </si>
+  <si>
+    <t>2022-05-21</t>
   </si>
 </sst>
 </file>
@@ -4950,7 +4968,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88F61A0-C462-45BA-9C2A-DB0E9A417211}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4962,14 +4980,16 @@
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>892</v>
       </c>
@@ -4989,22 +5009,28 @@
         <v>895</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>1088</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>897</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>950</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>968</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -5030,18 +5056,24 @@
       <c r="H2" s="1" t="s">
         <v>934</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="K2" s="1">
         <f>E2*2</f>
         <v>3600000</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -5062,23 +5094,29 @@
         <v>924</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>937</v>
+        <v>1085</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>938</v>
       </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I12" si="0">E3*2</f>
+      <c r="I3" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K12" si="0">E3*2</f>
         <v>2600000</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -5104,18 +5142,24 @@
       <c r="H4" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="K4" s="1">
         <f t="shared" si="0"/>
         <v>1100000</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -5141,18 +5185,24 @@
       <c r="H5" s="1" t="s">
         <v>933</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="K5" s="1">
         <f t="shared" si="0"/>
         <v>2900000</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -5173,23 +5223,29 @@
         <v>929</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>932</v>
+        <v>947</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="K6" s="1">
         <f>E6*2+479000</f>
         <v>2739000</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -5215,18 +5271,24 @@
       <c r="H7" s="1" t="s">
         <v>937</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
         <v>2300000</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -5250,20 +5312,26 @@
         <v>933</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="I8" s="1">
+      <c r="K8" s="1">
         <f>E8*2+1148000</f>
         <v>3748000</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -5289,18 +5357,24 @@
       <c r="H9" s="1" t="s">
         <v>940</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="K9" s="1">
         <f t="shared" si="0"/>
         <v>1900000</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -5326,18 +5400,24 @@
       <c r="H10" s="1" t="s">
         <v>945</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="K10" s="1">
         <f>E10*2+948000+70000</f>
         <v>3318000</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -5363,18 +5443,24 @@
       <c r="H11" s="1" t="s">
         <v>943</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="0"/>
         <v>1650000</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>1053</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -5398,20 +5484,26 @@
         <v>941</v>
       </c>
       <c r="H12" s="1" t="s">
+        <v>1086</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="I12" s="1">
+      <c r="K12" s="1">
         <f t="shared" si="0"/>
         <v>1610000</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -5432,22 +5524,28 @@
         <v>931</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>963</v>
+        <v>1087</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>963</v>
+        <v>1086</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>963</v>
       </c>
       <c r="J13" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="1">
+      <c r="M13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -5471,20 +5569,26 @@
         <v>935</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="I14" s="1">
+      <c r="K14" s="1">
         <f>E14*2+338000+248000</f>
         <v>9686000</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -5508,20 +5612,26 @@
         <v>935</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="I15" s="1">
+      <c r="K15" s="1">
         <f>E15*2+50000</f>
         <v>9150000</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -5545,16 +5655,22 @@
         <v>935</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>963</v>
       </c>
-      <c r="I16" s="1">
+      <c r="K16" s="1">
         <f>E16*2+406000+40000+278000</f>
         <v>9824000</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>